<commit_message>
2nd Sunday of Advent
</commit_message>
<xml_diff>
--- a/Vesperale OP English Psalm Tones.xlsx
+++ b/Vesperale OP English Psalm Tones.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Mode</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>(hr f) †(;3) (hr i h) &lt;v&gt;$\star$&lt;/v&gt;(;) (hr i g f ::)</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>(hr g) †(;3) (hr ixi g h) &lt;v&gt;$\star$&lt;/v&gt;(;) (hr g f g ::)</t>
   </si>
 </sst>
 </file>
@@ -386,7 +392,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,6 +417,26 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>5</v>

</xml_diff>